<commit_message>
added emx2 extensions option to profiles
</commit_message>
<xml_diff>
--- a/dist/umdm_lookups_emx2.xlsx
+++ b/dist/umdm_lookups_emx2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="127">
   <si>
     <t>attributeTemplateDefault</t>
   </si>
@@ -94,6 +94,18 @@
     <t>subjectStatus</t>
   </si>
   <si>
+    <t>subjects</t>
+  </si>
+  <si>
+    <t>samples</t>
+  </si>
+  <si>
+    <t>samplePreparation</t>
+  </si>
+  <si>
+    <t>sequencing</t>
+  </si>
+  <si>
     <t>value</t>
   </si>
   <si>
@@ -109,97 +121,133 @@
     <t>iri</t>
   </si>
   <si>
+    <t>linkedClinicalRecords</t>
+  </si>
+  <si>
+    <t>linkedSamples</t>
+  </si>
+  <si>
+    <t>linkedFiles</t>
+  </si>
+  <si>
+    <t>linkedSamplePreparations</t>
+  </si>
+  <si>
+    <t>linkedSequences</t>
+  </si>
+  <si>
     <t>string</t>
   </si>
   <si>
     <t>text</t>
   </si>
   <si>
-    <t>NCIT_C45677 http://purl.obolibrary.org/obo/NCIT_C45677</t>
-  </si>
-  <si>
-    <t>NCIT_C49100 http://purl.obolibrary.org/obo/NCIT_C49100</t>
-  </si>
-  <si>
-    <t>NCIT_C25365 http://purl.obolibrary.org/obo/NCIT_C25365</t>
-  </si>
-  <si>
-    <t>NCIT_C70895 http://purl.obolibrary.org/obo/NCIT_C70895</t>
-  </si>
-  <si>
-    <t>NCIT_C25162 http://purl.obolibrary.org/obo/NCIT_C25162</t>
-  </si>
-  <si>
-    <t>NCIT_C165071 http://purl.obolibrary.org/obo/NCIT_C165071</t>
-  </si>
-  <si>
-    <t>NCIT_C103264 http://purl.obolibrary.org/obo/NCIT_C103264</t>
-  </si>
-  <si>
-    <t>NCIT_C176763 http://purl.obolibrary.org/obo/NCIT_C176763</t>
-  </si>
-  <si>
-    <t>NCIT_C70713 http://purl.obolibrary.org/obo/NCIT_C70713</t>
-  </si>
-  <si>
-    <t>NCIT_C171105 http://purl.obolibrary.org/obo/NCIT_C171105</t>
-  </si>
-  <si>
-    <t>DUO_0000001 http://purl.obolibrary.org/obo/DUO_0000001</t>
-  </si>
-  <si>
-    <t>SNOMEDCT_723506003 http://purl.bioontology.org/ontology/SNOMEDCT/723506003</t>
-  </si>
-  <si>
-    <t>NCIT_C15607 http://purl.obolibrary.org/obo/NCIT_C15607</t>
-  </si>
-  <si>
-    <t>NCIT_C171193 http://purl.obolibrary.org/obo/NCIT_C171193</t>
-  </si>
-  <si>
-    <t>EDAM_2340 http://edamontology.org/data_2340</t>
-  </si>
-  <si>
-    <t>MESH_D005783 http://purl.bioontology.org/ontology/MESH/D005783</t>
-  </si>
-  <si>
-    <t>GSSO_009418 http://purl.obolibrary.org/obo/GSSO_009418</t>
-  </si>
-  <si>
-    <t>PATO_0020000 http://purl.obolibrary.org/obo/PATO_0020000</t>
-  </si>
-  <si>
-    <t>OBI_0500027 http://purl.obolibrary.org/obo/OBI_0500027</t>
-  </si>
-  <si>
-    <t>NCIT_C20826 http://purl.obolibrary.org/obo/NCIT_C20826</t>
-  </si>
-  <si>
-    <t>GENEPIO_0000085 http://purl.obolibrary.org/obo/GENEPIO_0000085</t>
-  </si>
-  <si>
-    <t>GO_0001894 http://purl.obolibrary.org/obo/GO_0001894</t>
-  </si>
-  <si>
-    <t>NCIT_C16977 http://purl.obolibrary.org/obo/NCIT_C16977</t>
-  </si>
-  <si>
-    <t>NCIT_C171003 http://purl.obolibrary.org/obo/NCIT_C171003</t>
-  </si>
-  <si>
-    <t>GENEPIO_0001921 http://purl.obolibrary.org/obo/GENEPIO_0001921</t>
-  </si>
-  <si>
-    <t>FIX_0000704 http://purl.obolibrary.org/obo/FIX_0000704</t>
-  </si>
-  <si>
-    <t>GENEPIO_0000071 http://purl.obolibrary.org/obo/GENEPIO_0000071</t>
-  </si>
-  <si>
-    <t>NCIT_C171103 http://purl.obolibrary.org/obo/NCIT_C171103</t>
-  </si>
-  <si>
-    <t>NCIT_C117655 http://purl.obolibrary.org/obo/NCIT_C117655</t>
+    <t>refBack</t>
+  </si>
+  <si>
+    <t>clinical</t>
+  </si>
+  <si>
+    <t>files</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C103264</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176763</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70713</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171105</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DUO_0000001</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/SNOMEDCT/723506003</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C15607</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171193</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_2340</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/MESH/D005783</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GSSO_009418</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/PATO_0020000</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0500027</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C20826</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0000085</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GO_0001894</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16977</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171003</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0001921</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/FIX_0000704</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0000071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171103</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C117655</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C87853</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_3273</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C132299</t>
   </si>
   <si>
     <t>attribute template where value is the primary key</t>
@@ -293,6 +341,30 @@
   </si>
   <si>
     <t>A findings domain that contains general subject characteristics that are evaluated periodically to determine if they have changed.</t>
+  </si>
+  <si>
+    <t>A unique proper name or character sequence that identifies this particular clinical examination.</t>
+  </si>
+  <si>
+    <t>Name or other identifier of an entry from a biosample database.</t>
+  </si>
+  <si>
+    <t>The literal identifier for an electronic file.</t>
+  </si>
+  <si>
+    <t>A unique proper name or character sequence that identifies this particular sample preparation.</t>
+  </si>
+  <si>
+    <t>belongsToSubject</t>
+  </si>
+  <si>
+    <t>belongsToSample</t>
+  </si>
+  <si>
+    <t>belongsToSamplePreparation</t>
+  </si>
+  <si>
+    <t>producedBySequencing</t>
   </si>
   <si>
     <t>tableName</t>
@@ -329,7 +401,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,6 +415,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -369,14 +448,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -669,67 +754,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
-        <v>33</v>
+      <c r="J2" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="K2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -737,152 +825,152 @@
       <c r="F3" t="b">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="K3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
       <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="K7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="J8" t="s">
-        <v>33</v>
+      <c r="J8" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="K8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="J9" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="K9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" t="s">
-        <v>35</v>
+        <v>41</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="K10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" t="s">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="K11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -890,70 +978,70 @@
       <c r="F12" t="b">
         <v>1</v>
       </c>
-      <c r="J12" t="s">
-        <v>37</v>
+      <c r="J12" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="K12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="K13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
-      <c r="J14" t="s">
-        <v>39</v>
+      <c r="J14" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="K14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
-      <c r="J15" t="s">
-        <v>40</v>
+      <c r="J15" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="K15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
       </c>
-      <c r="J16" t="s">
-        <v>41</v>
+      <c r="J16" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="K16" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -963,11 +1051,11 @@
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="J17" t="s">
-        <v>42</v>
+      <c r="J17" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="K17" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -977,11 +1065,11 @@
       <c r="B18" t="s">
         <v>0</v>
       </c>
-      <c r="J18" t="s">
-        <v>43</v>
+      <c r="J18" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="K18" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -991,11 +1079,11 @@
       <c r="B19" t="s">
         <v>0</v>
       </c>
-      <c r="J19" t="s">
-        <v>43</v>
+      <c r="J19" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="K19" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1005,11 +1093,11 @@
       <c r="B20" t="s">
         <v>0</v>
       </c>
-      <c r="J20" t="s">
-        <v>44</v>
+      <c r="J20" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="K20" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1019,11 +1107,11 @@
       <c r="B21" t="s">
         <v>0</v>
       </c>
-      <c r="J21" t="s">
-        <v>45</v>
+      <c r="J21" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="K21" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1033,11 +1121,11 @@
       <c r="B22" t="s">
         <v>0</v>
       </c>
-      <c r="J22" t="s">
-        <v>46</v>
+      <c r="J22" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="K22" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1047,11 +1135,11 @@
       <c r="B23" t="s">
         <v>0</v>
       </c>
-      <c r="J23" t="s">
-        <v>47</v>
+      <c r="J23" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="K23" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1061,11 +1149,11 @@
       <c r="B24" t="s">
         <v>0</v>
       </c>
-      <c r="J24" t="s">
-        <v>48</v>
+      <c r="J24" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="K24" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1075,11 +1163,11 @@
       <c r="B25" t="s">
         <v>0</v>
       </c>
-      <c r="J25" t="s">
-        <v>49</v>
+      <c r="J25" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="K25" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1089,11 +1177,11 @@
       <c r="B26" t="s">
         <v>0</v>
       </c>
-      <c r="J26" t="s">
-        <v>50</v>
+      <c r="J26" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="K26" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1103,11 +1191,11 @@
       <c r="B27" t="s">
         <v>0</v>
       </c>
-      <c r="J27" t="s">
-        <v>51</v>
+      <c r="J27" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="K27" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1117,11 +1205,11 @@
       <c r="B28" t="s">
         <v>0</v>
       </c>
-      <c r="J28" t="s">
-        <v>52</v>
+      <c r="J28" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="K28" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1131,11 +1219,11 @@
       <c r="B29" t="s">
         <v>0</v>
       </c>
-      <c r="J29" t="s">
-        <v>53</v>
+      <c r="J29" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="K29" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1145,11 +1233,11 @@
       <c r="B30" t="s">
         <v>0</v>
       </c>
-      <c r="J30" t="s">
-        <v>54</v>
+      <c r="J30" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="K30" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1159,11 +1247,11 @@
       <c r="B31" t="s">
         <v>1</v>
       </c>
-      <c r="J31" t="s">
-        <v>55</v>
+      <c r="J31" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="K31" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1173,84 +1261,266 @@
       <c r="B32" t="s">
         <v>0</v>
       </c>
-      <c r="J32" t="s">
-        <v>56</v>
+      <c r="J32" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="K32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>21</v>
       </c>
       <c r="B33" t="s">
         <v>0</v>
       </c>
-      <c r="J33" t="s">
-        <v>57</v>
+      <c r="J33" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="K33" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>22</v>
       </c>
       <c r="B34" t="s">
         <v>0</v>
       </c>
-      <c r="J34" t="s">
-        <v>58</v>
+      <c r="J34" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="K34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>23</v>
       </c>
       <c r="B35" t="s">
         <v>0</v>
       </c>
-      <c r="J35" t="s">
-        <v>59</v>
+      <c r="J35" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="K35" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>24</v>
       </c>
       <c r="B36" t="s">
         <v>0</v>
       </c>
-      <c r="J36" t="s">
-        <v>60</v>
+      <c r="J36" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="K36" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>25</v>
       </c>
       <c r="B37" t="s">
         <v>0</v>
       </c>
-      <c r="J37" t="s">
-        <v>61</v>
+      <c r="J37" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="K37" t="s">
-        <v>92</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" t="s">
+        <v>42</v>
+      </c>
+      <c r="H38" t="s">
+        <v>43</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K38" t="s">
+        <v>109</v>
+      </c>
+      <c r="L38" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" t="s">
+        <v>42</v>
+      </c>
+      <c r="H39" t="s">
+        <v>27</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K39" t="s">
+        <v>110</v>
+      </c>
+      <c r="L39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" t="s">
+        <v>42</v>
+      </c>
+      <c r="H40" t="s">
+        <v>44</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K40" t="s">
+        <v>111</v>
+      </c>
+      <c r="L40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" t="s">
+        <v>42</v>
+      </c>
+      <c r="H41" t="s">
+        <v>28</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K41" t="s">
+        <v>110</v>
+      </c>
+      <c r="L41" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" t="s">
+        <v>42</v>
+      </c>
+      <c r="H42" t="s">
+        <v>29</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K42" t="s">
+        <v>112</v>
+      </c>
+      <c r="L42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" t="s">
+        <v>42</v>
+      </c>
+      <c r="H43" t="s">
+        <v>44</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K43" t="s">
+        <v>111</v>
+      </c>
+      <c r="L43" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="J4" r:id="rId3"/>
+    <hyperlink ref="J5" r:id="rId4"/>
+    <hyperlink ref="J6" r:id="rId5"/>
+    <hyperlink ref="J7" r:id="rId6"/>
+    <hyperlink ref="J8" r:id="rId7"/>
+    <hyperlink ref="J9" r:id="rId8"/>
+    <hyperlink ref="J10" r:id="rId9"/>
+    <hyperlink ref="J11" r:id="rId10"/>
+    <hyperlink ref="J12" r:id="rId11"/>
+    <hyperlink ref="J13" r:id="rId12"/>
+    <hyperlink ref="J14" r:id="rId13"/>
+    <hyperlink ref="J15" r:id="rId14"/>
+    <hyperlink ref="J16" r:id="rId15"/>
+    <hyperlink ref="J17" r:id="rId16"/>
+    <hyperlink ref="J18" r:id="rId17"/>
+    <hyperlink ref="J19" r:id="rId18"/>
+    <hyperlink ref="J20" r:id="rId19"/>
+    <hyperlink ref="J21" r:id="rId20"/>
+    <hyperlink ref="J22" r:id="rId21"/>
+    <hyperlink ref="J23" r:id="rId22"/>
+    <hyperlink ref="J24" r:id="rId23"/>
+    <hyperlink ref="J25" r:id="rId24"/>
+    <hyperlink ref="J26" r:id="rId25"/>
+    <hyperlink ref="J27" r:id="rId26"/>
+    <hyperlink ref="J28" r:id="rId27"/>
+    <hyperlink ref="J29" r:id="rId28"/>
+    <hyperlink ref="J30" r:id="rId29"/>
+    <hyperlink ref="J31" r:id="rId30"/>
+    <hyperlink ref="J32" r:id="rId31"/>
+    <hyperlink ref="J33" r:id="rId32"/>
+    <hyperlink ref="J34" r:id="rId33"/>
+    <hyperlink ref="J35" r:id="rId34"/>
+    <hyperlink ref="J36" r:id="rId35"/>
+    <hyperlink ref="J37" r:id="rId36"/>
+    <hyperlink ref="J38" r:id="rId37"/>
+    <hyperlink ref="J39" r:id="rId38"/>
+    <hyperlink ref="J40" r:id="rId39"/>
+    <hyperlink ref="J41" r:id="rId40"/>
+    <hyperlink ref="J42" r:id="rId41"/>
+    <hyperlink ref="J43" r:id="rId42"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>